<commit_message>
SoCDTtiNTY calibration for passenger LDVs
</commit_message>
<xml_diff>
--- a/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
+++ b/InputData/trans/SoCDTtiNTY/Share of Cargo Dist Transported that is New This Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/nathaniyer/library/containers/com.microsoft.excel/data/state-eps-data-repository/template_state/trans/socdttinty/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-oregon\InputData\trans\SoCDTtiNTY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7277D8F6-8D33-D949-9D28-686E49FD3DCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE97D2E0-44AF-4F08-B6ED-0EC45B9D4244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -680,9 +680,9 @@
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
         <v>44307</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -698,72 +698,72 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
@@ -777,23 +777,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E6D016D-4C71-824D-8201-BB75DC201208}">
   <dimension ref="A2:AG85"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="79.5" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="1" max="1" width="79.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -802,7 +802,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -814,7 +814,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -826,7 +826,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -838,7 +838,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -850,7 +850,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -862,7 +862,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -875,7 +875,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -888,7 +888,7 @@
       </c>
       <c r="D9" s="6"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -901,7 +901,7 @@
       </c>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -914,7 +914,7 @@
       </c>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -927,7 +927,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -940,7 +940,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -953,12 +953,12 @@
       </c>
       <c r="D14" s="6"/>
     </row>
-    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -984,7 +984,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>13</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>16</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>17</v>
       </c>
@@ -1140,12 +1140,12 @@
         <v>5.8823529411764705E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>13</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>14</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>15</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>16</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>17</v>
       </c>
@@ -1327,12 +1327,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>26</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>40</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>431079</v>
       </c>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>41</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>19365</v>
       </c>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>42</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>43</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>9906</v>
       </c>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>44</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>45</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>46</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>47</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>48</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>18263</v>
       </c>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>49</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>50</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>14229</v>
       </c>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>51</v>
       </c>
@@ -2645,15 +2645,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="9"/>
     </row>
-    <row r="52" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>40</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>7.0636704641144667E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>41</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>1.1773818745158792E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>42</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>1.1538461538461539E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>43</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>4.6638400969109629E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>44</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>45</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59" s="13" t="s">
         <v>46</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>47</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>48</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>49</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:33" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>50</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>-1.0752688172043012E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64" s="13" t="s">
         <v>51</v>
       </c>
@@ -4024,12 +4024,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>18</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>12</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>7.5544641465039475E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>13</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>14</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>15</v>
       </c>
@@ -4166,7 +4166,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>16</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>17</v>
       </c>
@@ -4225,12 +4225,12 @@
         <v>5.819624978580696E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>18</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>12</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>7.1570453134698939E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>13</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>14</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>15</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>16</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>17</v>
       </c>
@@ -4432,16 +4432,16 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="8" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -4467,40 +4467,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2">
-        <f>'Calibration Helper'!B70</f>
-        <v>7.5544641465039475E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="C2">
-        <f>'Calibration Helper'!C70</f>
-        <v>7.5544641465039475E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="D2">
-        <f>'Calibration Helper'!D70</f>
-        <v>7.5544641465039475E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E2">
-        <f>'Calibration Helper'!E70</f>
-        <v>7.5544641465039475E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="F2">
-        <f>'Calibration Helper'!F70</f>
-        <v>7.5544641465039475E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="G2">
-        <f>'Calibration Helper'!G70</f>
-        <v>7.5544641465039475E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="H2">
-        <f>'Calibration Helper'!H70</f>
-        <v>7.5544641465039475E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7.8E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4533,7 +4526,7 @@
         <v>4.3478260869565216E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4566,7 +4559,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4599,7 +4592,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -4632,7 +4625,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -4681,13 +4674,13 @@
       <selection activeCell="B2" sqref="B2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="8" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -4713,7 +4706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4746,7 +4739,7 @@
         <v>7.1570453134698939E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -4779,7 +4772,7 @@
         <v>3.5714285714285712E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4812,7 +4805,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -4845,7 +4838,7 @@
         <v>2.9411764705882353E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -4878,7 +4871,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>

</xml_diff>